<commit_message>
first completly working model
</commit_message>
<xml_diff>
--- a/TransmitionDiagram.xlsx
+++ b/TransmitionDiagram.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="39">
   <si>
     <t>Byte</t>
   </si>
@@ -103,9 +103,6 @@
     <t>NEW_TRASMITION_HEADER_B3</t>
   </si>
   <si>
-    <t>NEW_TRASMITION_HEADER_B4</t>
-  </si>
-  <si>
     <t>STOP_SEQUENCE_B3</t>
   </si>
   <si>
@@ -121,9 +118,6 @@
     <t>TRASMITION_HEADER_B3</t>
   </si>
   <si>
-    <t>TRASMITION_HEADER_B4</t>
-  </si>
-  <si>
     <t>FINAL_STOP_SEQUENCE_B1</t>
   </si>
   <si>
@@ -134,6 +128,12 @@
   </si>
   <si>
     <t>FINAL_STOP_SEQUENCE_B4</t>
+  </si>
+  <si>
+    <t>SEQUENCE_ID_SIZE + CAP_VOLTAGE_SIZE + ESTIMATED_ENERGY_QUALITY_SIZE+  DATA_SIZE</t>
+  </si>
+  <si>
+    <t>TRASMIT_SECTOR_B0</t>
   </si>
 </sst>
 </file>
@@ -166,7 +166,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +215,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="8">
     <border>
@@ -329,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -379,6 +385,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -676,7 +686,7 @@
   <dimension ref="A3:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -800,13 +810,13 @@
         <v>2</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13" s="5">
         <v>2</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -821,34 +831,34 @@
         <v>3</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J14" s="5">
         <v>3</v>
       </c>
       <c r="K14" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
-      <c r="D15" s="5">
+      <c r="D15" s="25">
         <v>4</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="5">
+      <c r="E15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="25">
         <v>4</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="J15" s="5">
+      <c r="H15" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" s="25">
         <v>4</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>34</v>
+      <c r="K15" s="26" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1264,7 +1274,7 @@
         <v>2061</v>
       </c>
       <c r="K33" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:11" ht="15.75" thickBot="1">
@@ -1275,19 +1285,19 @@
         <v>2062</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G34" s="20">
         <v>2062</v>
       </c>
       <c r="H34" s="21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J34" s="20">
         <v>2062</v>
       </c>
       <c r="K34" s="19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="15.75" thickBot="1">
@@ -1298,19 +1308,19 @@
         <v>2063</v>
       </c>
       <c r="E35" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G35" s="20">
         <v>2063</v>
       </c>
       <c r="H35" s="21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J35" s="20">
         <v>2063</v>
       </c>
       <c r="K35" s="19" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="15.75" thickBot="1">
@@ -1321,19 +1331,24 @@
         <v>2064</v>
       </c>
       <c r="E36" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G36" s="20">
         <v>2064</v>
       </c>
       <c r="H36" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J36" s="20">
         <v>2064</v>
       </c>
       <c r="K36" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="E39" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:11">

</xml_diff>

<commit_message>
fixing start and end constants
</commit_message>
<xml_diff>
--- a/TransmitionDiagram.xlsx
+++ b/TransmitionDiagram.xlsx
@@ -12,12 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="43">
   <si>
     <t>Byte</t>
   </si>
@@ -130,17 +129,29 @@
     <t>FINAL_STOP_SEQUENCE_B4</t>
   </si>
   <si>
-    <t>SEQUENCE_ID_SIZE + CAP_VOLTAGE_SIZE + ESTIMATED_ENERGY_QUALITY_SIZE+  DATA_SIZE</t>
-  </si>
-  <si>
     <t>TRASMIT_SECTOR_B0</t>
+  </si>
+  <si>
+    <t>PGA_GAIN_SIZE</t>
+  </si>
+  <si>
+    <t>FREE_0</t>
+  </si>
+  <si>
+    <t>FREE_1</t>
+  </si>
+  <si>
+    <t>FREE_2</t>
+  </si>
+  <si>
+    <t>FREE_3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +176,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,8 +239,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -331,11 +355,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -366,10 +405,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,6 +422,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -683,10 +729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:K43"/>
+  <dimension ref="A3:K41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -735,24 +781,24 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" s="1"/>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E10" s="23" t="s">
+      <c r="E10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="24"/>
-      <c r="G10" s="22" t="s">
+      <c r="F10" s="22"/>
+      <c r="G10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="H10" s="23" t="s">
+      <c r="H10" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="22" t="s">
+      <c r="I10" s="22"/>
+      <c r="J10" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="K10" s="23" t="s">
+      <c r="K10" s="21" t="s">
         <v>22</v>
       </c>
     </row>
@@ -842,23 +888,23 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="1"/>
-      <c r="D15" s="25">
+      <c r="D15" s="23">
         <v>4</v>
       </c>
-      <c r="E15" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="25">
+      <c r="E15" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="23">
         <v>4</v>
       </c>
-      <c r="H15" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="J15" s="25">
+      <c r="H15" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="J15" s="23">
         <v>4</v>
       </c>
-      <c r="K15" s="26" t="s">
-        <v>38</v>
+      <c r="K15" s="24" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1189,173 +1235,262 @@
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
-      <c r="D30" s="16">
+      <c r="D30" s="25">
         <v>2058</v>
       </c>
-      <c r="E30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G30" s="16">
+      <c r="E30" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="25">
         <v>2058</v>
       </c>
-      <c r="H30" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="J30" s="16">
+      <c r="H30" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="J30" s="25">
         <v>2058</v>
       </c>
-      <c r="K30" s="17" t="s">
-        <v>11</v>
+      <c r="K30" s="26" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
-      <c r="D31" s="16">
+      <c r="D31" s="27">
         <v>2059</v>
       </c>
-      <c r="E31" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="16">
+      <c r="E31" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="27">
         <v>2059</v>
       </c>
-      <c r="H31" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="J31" s="16">
+      <c r="H31" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" s="27">
         <v>2059</v>
       </c>
-      <c r="K31" s="17" t="s">
-        <v>12</v>
+      <c r="K31" s="26" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
-      <c r="D32" s="18">
+      <c r="D32" s="25">
         <v>2060</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="G32" s="18">
+      <c r="E32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="25">
         <v>2060</v>
       </c>
-      <c r="H32" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="J32" s="18">
+      <c r="H32" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="25">
         <v>2060</v>
       </c>
-      <c r="K32" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K32" s="26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
-      <c r="D33" s="20">
+      <c r="D33" s="27">
         <v>2061</v>
       </c>
-      <c r="E33" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="G33" s="20">
+      <c r="E33" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G33" s="27">
         <v>2061</v>
       </c>
-      <c r="H33" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="J33" s="20">
+      <c r="H33" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="27">
         <v>2061</v>
       </c>
-      <c r="K33" s="19" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K33" s="26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
-      <c r="D34" s="20">
+      <c r="D34" s="25">
         <v>2062</v>
       </c>
-      <c r="E34" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="G34" s="20">
+      <c r="E34" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="25">
         <v>2062</v>
       </c>
-      <c r="H34" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="J34" s="20">
+      <c r="H34" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J34" s="25">
         <v>2062</v>
       </c>
-      <c r="K34" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K34" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
-      <c r="D35" s="20">
+      <c r="D35" s="28">
         <v>2063</v>
       </c>
-      <c r="E35" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="G35" s="20">
+      <c r="E35" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="28">
         <v>2063</v>
       </c>
-      <c r="H35" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="J35" s="20">
+      <c r="H35" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" s="28">
         <v>2063</v>
       </c>
-      <c r="K35" s="19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1">
+      <c r="K35" s="29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
-      <c r="D36" s="20">
+      <c r="D36" s="28">
         <v>2064</v>
       </c>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="28">
+        <v>2064</v>
+      </c>
+      <c r="H36" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="J36" s="28">
+        <v>2064</v>
+      </c>
+      <c r="K36" s="29" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="D37" s="16">
+        <v>2065</v>
+      </c>
+      <c r="E37" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G37" s="16">
+        <v>2065</v>
+      </c>
+      <c r="H37" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="J37" s="16">
+        <v>2065</v>
+      </c>
+      <c r="K37" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="15.75" thickBot="1">
+      <c r="D38" s="18">
+        <v>2066</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G38" s="18">
+        <v>2066</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J38" s="18">
+        <v>2066</v>
+      </c>
+      <c r="K38" s="17" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="15.75" thickBot="1">
+      <c r="D39" s="16">
+        <v>2067</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="16">
+        <v>2067</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="16">
+        <v>2067</v>
+      </c>
+      <c r="K39" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="15.75" thickBot="1">
+      <c r="D40" s="18">
+        <v>2068</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="G40" s="18">
+        <v>2068</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="J40" s="18">
+        <v>2068</v>
+      </c>
+      <c r="K40" s="17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="15.75" thickBot="1">
+      <c r="D41" s="16">
+        <v>2069</v>
+      </c>
+      <c r="E41" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="20">
-        <v>2064</v>
-      </c>
-      <c r="H36" s="21" t="s">
+      <c r="G41" s="16">
+        <v>2069</v>
+      </c>
+      <c r="H41" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="J36" s="20">
-        <v>2064</v>
-      </c>
-      <c r="K36" s="19" t="s">
+      <c r="J41" s="16">
+        <v>2069</v>
+      </c>
+      <c r="K41" s="17" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="E39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="K42" s="19"/>
-    </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1">
-      <c r="K43" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>